<commit_message>
Add Access Key support
</commit_message>
<xml_diff>
--- a/s3IAMCommands.xlsx
+++ b/s3IAMCommands.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27930"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wasabicloud.sharepoint.com/sites/WasabiJapanSite/SE  Engineering/Opportunities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="136" documentId="13_ncr:1_{ECE4C5F1-FFD4-4552-8499-DAFE11FDED2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F402DFC-2CC7-492B-9A5D-B7404DFF10D4}"/>
+  <xr:revisionPtr revIDLastSave="214" documentId="13_ncr:1_{ECE4C5F1-FFD4-4552-8499-DAFE11FDED2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D07A4FE3-7055-4F7B-B9B1-92D28B5163ED}"/>
   <bookViews>
-    <workbookView xWindow="12820" yWindow="6150" windowWidth="22750" windowHeight="13320" firstSheet="9" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12820" yWindow="6150" windowWidth="22750" windowHeight="13320" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="11" r:id="rId1"/>
@@ -23,6 +23,8 @@
     <sheet name="RemoveUserFromGroup" sheetId="12" r:id="rId8"/>
     <sheet name="DeleteLoginProfile" sheetId="7" r:id="rId9"/>
     <sheet name="DeleteUsers" sheetId="10" r:id="rId10"/>
+    <sheet name="CreateUserAccessKeys" sheetId="14" r:id="rId11"/>
+    <sheet name="DeleteUserAccessKeys" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="279">
   <si>
     <t>This Spreadsheet is prepared to automate the operation related to IAM such as manage users and groups.</t>
   </si>
@@ -131,10 +133,10 @@
     <t>AWS CLI Configuration and Credential File作成</t>
   </si>
   <si>
-    <t xml:space="preserve">AWS CLI 設定および認証情報ファイル コマンドを実行するには、アクセスキーとシークレットキーを使用してAWS CLIを設定する必要があります。 </t>
-  </si>
-  <si>
-    <t>設定ファイルと認証情報ファイルは、”aws configure” コマンドを実行することで、AWS CLI をインストールした状態で作成できます。</t>
+    <t>AWS CLIコマンドを実行するには、アクセスキーとシークレットキーを指定した設定ファイルと認証情報ファイルを作成する必要があります。</t>
+  </si>
+  <si>
+    <t>設定ファイルと認証情報ファイルは、”aws configure” コマンドを実行することで作成され、AWS CLI のインストールが必要となります。</t>
   </si>
   <si>
     <t xml:space="preserve"> aws 設定 詳細については、このAWSドキュメントを参照してください。</t>
@@ -161,148 +163,166 @@
     <t>エンドポイントは必ず「--endpoint-url https://iam.ap-northeast-1.wasabisys.com」を追加してください(必要に応じて対象地域に応じて変更してください)</t>
   </si>
   <si>
+    <t>user1@gakunin.edu</t>
+  </si>
+  <si>
+    <t>aws iam create-user --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name</t>
+  </si>
+  <si>
+    <t>user2@gakunin.edu</t>
+  </si>
+  <si>
+    <t>user3@gakunin.edu</t>
+  </si>
+  <si>
+    <t>user4@gakunin.edu</t>
+  </si>
+  <si>
+    <t>user5@gakunin.edu</t>
+  </si>
+  <si>
+    <t>user6@gakunin.edu</t>
+  </si>
+  <si>
+    <t>https://awscli.amazonaws.com/v2/documentation/api/latest/reference/iam/create-user.html</t>
+  </si>
+  <si>
+    <t>aws iam create-user --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name USERNAME</t>
+  </si>
+  <si>
+    <t>NOTE: aws iam list-users --endpoint https://iam.ap-northeast-1.wasabisys.com</t>
+  </si>
+  <si>
+    <t>aws iam create-user help</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>***********</t>
+  </si>
+  <si>
+    <t>Creates a new IAM user for your Amazon Web Services account.</t>
+  </si>
+  <si>
+    <t>For information about quotas for the number of IAM users you can</t>
+  </si>
+  <si>
+    <t>create, see IAM and STS quotas in the *IAM User Guide* .</t>
+  </si>
+  <si>
+    <t>See also: AWS API Documentation</t>
+  </si>
+  <si>
+    <t>Synopsis</t>
+  </si>
+  <si>
+    <t>********</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     create-user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [--path &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   --user-name &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [--permissions-boundary &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [--tags &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [--cli-input-json | --cli-input-yaml]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [--generate-cli-skeleton &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [--debug]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [--endpoint-url &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [--no-verify-ssl]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [--no-paginate]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [--output &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [--query &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [--profile &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [--region &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [--version &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [--color &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [--no-sign-request]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [--ca-bundle &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [--cli-read-timeout &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [--cli-connect-timeout &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [--cli-binary-format &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [--no-cli-pager]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [--cli-auto-prompt]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [--no-cli-auto-prompt]</t>
+  </si>
+  <si>
     <t>GakuninUser1</t>
   </si>
   <si>
-    <t>aws iam create-user --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name</t>
+    <t>Password1</t>
+  </si>
+  <si>
+    <t>aws iam create-login-profile --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name</t>
   </si>
   <si>
     <t>GakuninUser2</t>
   </si>
   <si>
+    <t>Password2</t>
+  </si>
+  <si>
     <t>GakuninUser3</t>
   </si>
   <si>
+    <t>Password3</t>
+  </si>
+  <si>
     <t>GakuninUser4</t>
   </si>
   <si>
+    <t>Password4</t>
+  </si>
+  <si>
     <t>GakuninUser5</t>
-  </si>
-  <si>
-    <t>https://awscli.amazonaws.com/v2/documentation/api/latest/reference/iam/create-user.html</t>
-  </si>
-  <si>
-    <t>aws iam create-user --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name USERNAME</t>
-  </si>
-  <si>
-    <t>NOTE: aws iam list-users --endpoint https://iam.ap-northeast-1.wasabisys.com</t>
-  </si>
-  <si>
-    <t>aws iam create-user help</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>***********</t>
-  </si>
-  <si>
-    <t>Creates a new IAM user for your Amazon Web Services account.</t>
-  </si>
-  <si>
-    <t>For information about quotas for the number of IAM users you can</t>
-  </si>
-  <si>
-    <t>create, see IAM and STS quotas in the *IAM User Guide* .</t>
-  </si>
-  <si>
-    <t>See also: AWS API Documentation</t>
-  </si>
-  <si>
-    <t>Synopsis</t>
-  </si>
-  <si>
-    <t>********</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     create-user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   [--path &lt;value&gt;]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   --user-name &lt;value&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   [--permissions-boundary &lt;value&gt;]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   [--tags &lt;value&gt;]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   [--cli-input-json | --cli-input-yaml]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   [--generate-cli-skeleton &lt;value&gt;]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   [--debug]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   [--endpoint-url &lt;value&gt;]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   [--no-verify-ssl]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   [--no-paginate]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   [--output &lt;value&gt;]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   [--query &lt;value&gt;]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   [--profile &lt;value&gt;]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   [--region &lt;value&gt;]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   [--version &lt;value&gt;]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   [--color &lt;value&gt;]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   [--no-sign-request]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   [--ca-bundle &lt;value&gt;]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   [--cli-read-timeout &lt;value&gt;]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   [--cli-connect-timeout &lt;value&gt;]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   [--cli-binary-format &lt;value&gt;]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   [--no-cli-pager]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   [--cli-auto-prompt]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   [--no-cli-auto-prompt]</t>
-  </si>
-  <si>
-    <t>Password1</t>
-  </si>
-  <si>
-    <t>aws iam create-login-profile --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name</t>
-  </si>
-  <si>
-    <t>Password2</t>
-  </si>
-  <si>
-    <t>Password3</t>
-  </si>
-  <si>
-    <t>Password4</t>
   </si>
   <si>
     <t>Password5</t>
@@ -740,6 +760,192 @@
   </si>
   <si>
     <t xml:space="preserve">     delete-user</t>
+  </si>
+  <si>
+    <t>aws iam create-access-key --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name</t>
+  </si>
+  <si>
+    <t>NOTE: User Has to be created</t>
+  </si>
+  <si>
+    <t>https://docs.aws.amazon.com/cli/latest/reference/iam/create-access-key.html</t>
+  </si>
+  <si>
+    <t>aws iam create-access-key --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name USERNAME</t>
+  </si>
+  <si>
+    <t>aws iam create-access-key help</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       Creates  a  new Amazon Web Services secret access key and corresponding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       Amazon Web Services access key ID for the specified user.  The  default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       status for new keys is Active .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       If you do not specify a user name, IAM determines the user name implic-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       itly based on the Amazon Web Services access key  ID  signing  the  re-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       quest.  This  operation works for access keys under the Amazon Web Ser-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       vices account. Consequently, you can use this operation to manage  Ama-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       zon  Web  Services  account root user credentials. This is true even if</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       the Amazon Web Services account has no associated users.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       For information about quotas on the number of keys you can create,  see</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       IAM and STS quotas in the IAM User Guide .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       WARNING:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          To  ensure the security of your Amazon Web Services account, the se-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          cret access key is accessible only during key and user creation. You</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          must  save  the  key (for example, in a text file) if you want to be</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          able to access it again. If a secret key is lost, you can delete the</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          access keys for the associated user and then create new keys.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       See also: AWS API Documentation</t>
+  </si>
+  <si>
+    <t>SYNOPSIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            create-access-key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          [--user-name &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          [--cli-input-json | --cli-input-yaml]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          [--generate-cli-skeleton &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          [--debug]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          [--endpoint-url &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          [--no-verify-ssl]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          [--no-paginate]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          [--output &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          [--query &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          [--profile &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          [--region &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          [--version &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          [--color &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          [--no-sign-request]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          [--ca-bundle &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          [--cli-read-timeout &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          [--cli-connect-timeout &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          [--cli-binary-format &lt;value&gt;]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          [--no-cli-pager]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          [--cli-auto-prompt]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          [--no-cli-auto-prompt]</t>
+  </si>
+  <si>
+    <t>AccessKey1</t>
+  </si>
+  <si>
+    <t>aws iam delete-access-key --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name</t>
+  </si>
+  <si>
+    <t>AccessKey2</t>
+  </si>
+  <si>
+    <t>AccessKey3</t>
+  </si>
+  <si>
+    <t>AccessKey4</t>
+  </si>
+  <si>
+    <t>AccessKey5</t>
+  </si>
+  <si>
+    <t>NOTE: User has to exist</t>
+  </si>
+  <si>
+    <t>https://docs.aws.amazon.com/cli/latest/reference/iam/delete-access-key.html</t>
+  </si>
+  <si>
+    <t>aws iam delete-access-key --user-name &lt;USERNAME&gt; --access-key-id &lt;ACCESS_KEY_ID&gt;</t>
+  </si>
+  <si>
+    <t>aws iam delete-access-key help</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       Deletes the access key pair associated with the specified IAM user.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       zon  Web  Services account root user credentials even if the Amazon Web</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       Services account has no associated users.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            delete-access-key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          --access-key-id &lt;value&gt;</t>
   </si>
 </sst>
 </file>
@@ -951,7 +1157,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -994,6 +1200,7 @@
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1280,9 +1487,9 @@
   </sheetPr>
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A35" sqref="A35"/>
+      <selection pane="topRight" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -1545,8 +1752,8 @@
   </sheetPr>
   <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -1558,10 +1765,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="13" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="C1" s="14" t="str">
         <f>B1&amp;" "&amp;A1</f>
@@ -1570,10 +1777,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="13" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="C2" s="14" t="str">
         <f t="shared" ref="C2:C5" si="0">B2&amp;" "&amp;A2</f>
@@ -1582,10 +1789,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="13" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="C3" s="14" t="str">
         <f t="shared" si="0"/>
@@ -1594,10 +1801,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="13" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="C4" s="14" t="str">
         <f t="shared" si="0"/>
@@ -1606,10 +1813,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="13" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="C5" s="14" t="str">
         <f t="shared" si="0"/>
@@ -1618,238 +1825,878 @@
     </row>
     <row r="7" spans="1:3" ht="18.600000000000001">
       <c r="A7" s="5" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="11" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18.600000000000001">
       <c r="A9" s="3" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="10" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A8" r:id="rId1" xr:uid="{1ED3EAB9-FDA9-45D8-9A3D-11F0BB65F95B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA86FB75-4B3E-4926-A020-3F872FA8885C}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:C67"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="90" customWidth="1"/>
+    <col min="3" max="3" width="87.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="14.45">
+      <c r="A1" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="C1" s="14" t="str">
+        <f>B1&amp;" "&amp;A1</f>
+        <v>aws iam create-access-key --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name GakuninUser1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14.45">
+      <c r="A2" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="C2" s="14" t="str">
+        <f t="shared" ref="C2:C5" si="0">B2&amp;" "&amp;A2</f>
+        <v>aws iam create-access-key --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name GakuninUser2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="14.45">
+      <c r="A3" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="C3" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>aws iam create-access-key --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name GakuninUser3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="14.45">
+      <c r="A4" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="C4" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>aws iam create-access-key --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name GakuninUser4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="14.45">
+      <c r="A5" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="C5" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>aws iam create-access-key --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name GakuninUser5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18.600000000000001">
+      <c r="A7" s="5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="11" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18.600000000000001">
+      <c r="A9" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="14.45">
+      <c r="A11" s="10" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="14.45">
+      <c r="A12" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="14.45">
+      <c r="A13" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="14.45">
+      <c r="A15" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="14.45"/>
+    <row r="17" spans="1:1" ht="14.45">
+      <c r="A17" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="14.45">
+      <c r="A18" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="14.45">
+      <c r="A19" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="14.45">
+      <c r="A21" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="14.45"/>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="14.45">
+      <c r="A25" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="14.45">
+      <c r="A27" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="14.45">
+      <c r="A29" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="14.45">
+      <c r="A31" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="14.45">
+      <c r="A32" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="14.45">
+      <c r="A34" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="14.45">
+      <c r="A36" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="14.45">
+      <c r="A38" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="14.45">
+      <c r="A40" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="14.45">
+      <c r="A43" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="14.45">
+      <c r="A44" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="14.45">
+      <c r="A46" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="14.45">
+      <c r="A47" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="14.45">
+      <c r="A48" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="14.45">
+      <c r="A49" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="14.45">
+      <c r="A50" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="14.45">
+      <c r="A51" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="14.45">
+      <c r="A52" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="14.45">
+      <c r="A53" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="14.45">
+      <c r="A54" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="14.45">
+      <c r="A55" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="14.45">
+      <c r="A56" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="14.45">
+      <c r="A57" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="14.45">
+      <c r="A58" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="14.45"/>
+    <row r="60" spans="1:1" ht="14.45"/>
+    <row r="61" spans="1:1" ht="14.45"/>
+    <row r="62" spans="1:1" ht="14.45"/>
+    <row r="63" spans="1:1" ht="14.45"/>
+    <row r="64" spans="1:1" ht="14.45"/>
+    <row r="65" ht="14.45"/>
+    <row r="66" ht="14.45"/>
+    <row r="67" ht="14.45"/>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A8" r:id="rId1" xr:uid="{B14759B2-E84F-4D5C-A511-6C7E65546896}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA10414-20D7-4E04-A820-D52836CA053C}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:E47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="108.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="87.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1" s="17" t="str">
+        <f>"--access-key-id"</f>
+        <v>--access-key-id</v>
+      </c>
+      <c r="E1" s="14" t="str">
+        <f>C1&amp;" "&amp;A1&amp;" "&amp;D1&amp;" "&amp;B1</f>
+        <v>aws iam delete-access-key --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name GakuninUser1 --access-key-id AccessKey1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="D2" s="17" t="str">
+        <f t="shared" ref="D2:D5" si="0">"--access-key-id"</f>
+        <v>--access-key-id</v>
+      </c>
+      <c r="E2" s="14" t="str">
+        <f t="shared" ref="E2:E5" si="1">C2&amp;" "&amp;A2&amp;" "&amp;D2&amp;" "&amp;B2</f>
+        <v>aws iam delete-access-key --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name GakuninUser2 --access-key-id AccessKey2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="D3" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>--access-key-id</v>
+      </c>
+      <c r="E3" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>aws iam delete-access-key --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name GakuninUser3 --access-key-id AccessKey3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="D4" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>--access-key-id</v>
+      </c>
+      <c r="E4" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>aws iam delete-access-key --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name GakuninUser4 --access-key-id AccessKey4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="D5" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>--access-key-id</v>
+      </c>
+      <c r="E5" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>aws iam delete-access-key --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name GakuninUser5 --access-key-id AccessKey5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18.75">
+      <c r="A7" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B7" s="5"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="B8" s="11"/>
+    </row>
+    <row r="9" spans="1:5" ht="19.5">
+      <c r="A9" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="B11" s="10"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>263</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A8" r:id="rId1" xr:uid="{21292E10-2C0D-4FD8-A873-19CD43ED7160}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1860,10 +2707,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C5"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -1873,8 +2720,8 @@
     <col min="3" max="3" width="87.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:3" ht="15">
+      <c r="A1" s="34" t="s">
         <v>38</v>
       </c>
       <c r="B1" s="15" t="s">
@@ -1882,11 +2729,11 @@
       </c>
       <c r="C1" s="14" t="str">
         <f>B1&amp;" "&amp;A1</f>
-        <v>aws iam create-user --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name GakuninUser1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="13" t="s">
+        <v>aws iam create-user --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name user1@gakunin.edu</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15">
+      <c r="A2" s="34" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="15" t="s">
@@ -1894,11 +2741,11 @@
       </c>
       <c r="C2" s="14" t="str">
         <f t="shared" ref="C2:C5" si="0">B2&amp;" "&amp;A2</f>
-        <v>aws iam create-user --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name GakuninUser2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="13" t="s">
+        <v>aws iam create-user --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name user2@gakunin.edu</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15">
+      <c r="A3" s="34" t="s">
         <v>41</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -1906,11 +2753,11 @@
       </c>
       <c r="C3" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>aws iam create-user --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name GakuninUser3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="13" t="s">
+        <v>aws iam create-user --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name user3@gakunin.edu</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15">
+      <c r="A4" s="34" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="15" t="s">
@@ -1918,11 +2765,11 @@
       </c>
       <c r="C4" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>aws iam create-user --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name GakuninUser4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="13" t="s">
+        <v>aws iam create-user --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name user4@gakunin.edu</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15">
+      <c r="A5" s="34" t="s">
         <v>43</v>
       </c>
       <c r="B5" s="15" t="s">
@@ -1930,34 +2777,41 @@
       </c>
       <c r="C5" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>aws iam create-user --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name GakuninUser5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="11" t="s">
+        <v>aws iam create-user --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name user5@gakunin.edu</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15">
+      <c r="A6" s="34" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="18.600000000000001">
-      <c r="A9" s="3" t="s">
+      <c r="B6" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="14" t="str">
+        <f>B6&amp;" "&amp;A6</f>
+        <v>aws iam create-user --endpoint-url https://iam.ap-northeast-1.wasabisys.com --user-name user6@gakunin.edu</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="11" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18.600000000000001">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18.600000000000001">
-      <c r="A11" s="5"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="10" t="s">
+      <c r="A11" s="5" t="s">
         <v>47</v>
       </c>
     </row>
+    <row r="12" spans="1:3" ht="18.600000000000001">
+      <c r="A12" s="5"/>
+    </row>
     <row r="13" spans="1:3">
-      <c r="A13" t="s">
+      <c r="A13" s="10" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1966,13 +2820,13 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1981,13 +2835,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="s">
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1996,8 +2850,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2121,10 +2975,20 @@
         <v>80</v>
       </c>
     </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A8" r:id="rId1" xr:uid="{13E6C85E-942F-4452-B862-FD1EDDD3F283}"/>
+    <hyperlink ref="A9" r:id="rId1" xr:uid="{13E6C85E-942F-4452-B862-FD1EDDD3F283}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{4C213FF6-E960-41B7-A2C2-57935FBD7D7B}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{FC732670-60AB-4BBE-81FB-741C37AE7DFC}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{C9CB60A4-1E8B-44A8-AB09-450ED7642403}"/>
+    <hyperlink ref="A5" r:id="rId5" xr:uid="{609662BA-16B8-4B3F-9D76-F2199D03EC53}"/>
+    <hyperlink ref="A6" r:id="rId6" xr:uid="{B6DD9DFA-8087-4804-AB8A-4BEBE08D60FF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2138,7 +3002,7 @@
   <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E5"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2152,13 +3016,13 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="13" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D1" s="15" t="str">
         <f>"--no-password-reset-required --password"</f>
@@ -2171,13 +3035,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="13" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D2" s="15" t="str">
         <f t="shared" ref="D2:D5" si="0">"--no-password-reset-required --password"</f>
@@ -2190,13 +3054,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="13" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>84</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>82</v>
       </c>
       <c r="D3" s="15" t="str">
         <f t="shared" si="0"/>
@@ -2209,13 +3073,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="13" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D4" s="15" t="str">
         <f t="shared" si="0"/>
@@ -2228,13 +3092,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="13" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D5" s="15" t="str">
         <f t="shared" si="0"/>
@@ -2247,214 +3111,214 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="11" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18.600000000000001">
       <c r="A9" s="4" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="10" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2485,10 +3349,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="13" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C1" s="14" t="str">
         <f>B1&amp;" "&amp;A1</f>
@@ -2497,10 +3361,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="13" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C2" s="14" t="str">
         <f t="shared" ref="C2:C5" si="0">B2&amp;" "&amp;A2</f>
@@ -2509,10 +3373,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="13" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C3" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2521,10 +3385,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="13" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C4" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2533,10 +3397,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="13" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C5" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2545,172 +3409,172 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="11" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18.600000000000001">
       <c r="A9" s="4" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="10" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2730,7 +3594,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2744,13 +3608,13 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="13" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="D1" s="16" t="str">
         <f>"--group-name"</f>
@@ -2763,13 +3627,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="13" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="D2" s="16" t="str">
         <f t="shared" ref="D2:D5" si="0">"--group-name"</f>
@@ -2782,13 +3646,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="13" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="D3" s="16" t="str">
         <f t="shared" si="0"/>
@@ -2801,13 +3665,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="13" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="D4" s="16" t="str">
         <f t="shared" si="0"/>
@@ -2820,13 +3684,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="13" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="D5" s="16" t="str">
         <f t="shared" si="0"/>
@@ -2839,162 +3703,162 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="11" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18.600000000000001">
       <c r="A9" s="4" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="10" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -3027,13 +3891,13 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="13" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="D1" s="16" t="str">
         <f>"--policy-arn arn:aws:iam::aws:policy/"</f>
@@ -3046,13 +3910,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="13" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="D2" s="16" t="str">
         <f t="shared" ref="D2:D5" si="0">"--policy-arn arn:aws:iam::aws:policy/"</f>
@@ -3065,13 +3929,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="13" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="D3" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3084,13 +3948,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="13" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="D4" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3103,13 +3967,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="13" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="D5" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3122,282 +3986,282 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="11" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18.600000000000001">
       <c r="A9" s="4" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="11" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="6" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="7" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="7" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="7" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="7" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="7" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="7" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="8" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="7" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="7" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="7" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="7" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="7" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="7" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="7" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="10" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -3416,8 +4280,8 @@
   </sheetPr>
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection sqref="A1:E5"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Z1" sqref="Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -3431,13 +4295,13 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="13" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D1" s="17" t="str">
         <f>"--no-password-reset-required --password"</f>
@@ -3450,13 +4314,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="13" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D2" s="17" t="str">
         <f t="shared" ref="D2:D5" si="0">"--no-password-reset-required --password"</f>
@@ -3469,13 +4333,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="13" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D3" s="17" t="str">
         <f t="shared" si="0"/>
@@ -3488,13 +4352,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="13" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D4" s="17" t="str">
         <f t="shared" si="0"/>
@@ -3507,13 +4371,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="13" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D5" s="17" t="str">
         <f t="shared" si="0"/>
@@ -3526,12 +4390,12 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="11" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18.600000000000001">
       <c r="A9" s="4" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18.600000000000001">
@@ -3539,187 +4403,187 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="10" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -3738,7 +4602,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53:C71"/>
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -3752,13 +4616,13 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="13" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="D1" s="16" t="str">
         <f>"--group-name"</f>
@@ -3771,13 +4635,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="13" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="D2" s="16" t="str">
         <f t="shared" ref="D2:D5" si="0">"--group-name"</f>
@@ -3790,13 +4654,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="13" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="D3" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3809,13 +4673,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="13" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="D4" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3828,13 +4692,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="13" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="D5" s="16" t="str">
         <f t="shared" si="0"/>
@@ -3847,162 +4711,162 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="11" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18.600000000000001">
       <c r="A9" s="4" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="10" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -4017,9 +4881,7 @@
   </sheetPr>
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
@@ -4030,10 +4892,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="13" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="C1" s="14" t="str">
         <f>B1&amp;" "&amp;A1</f>
@@ -4042,10 +4904,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="13" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="C2" s="14" t="str">
         <f t="shared" ref="C2:C5" si="0">B2&amp;" "&amp;A2</f>
@@ -4054,10 +4916,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="13" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="C3" s="14" t="str">
         <f t="shared" si="0"/>
@@ -4066,10 +4928,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="13" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="C4" s="14" t="str">
         <f t="shared" si="0"/>
@@ -4078,10 +4940,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="13" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="C5" s="14" t="str">
         <f t="shared" si="0"/>
@@ -4090,218 +4952,218 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="11" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18.600000000000001">
       <c r="A9" s="4" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="10" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:1" s="2" customFormat="1">
       <c r="A36" s="2" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
     <row r="37" spans="1:1" s="2" customFormat="1">
       <c r="A37" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -4313,19 +5175,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d3c0bec9-ac84-4257-9162-9ea5559110db">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="57e54fb0-325f-4058-8825-bc3f38f5210f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010092D0BEC079D6A24EA52990B6802652F9" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f936298282562a7feddc828d2867168b">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d3c0bec9-ac84-4257-9162-9ea5559110db" xmlns:ns3="57e54fb0-325f-4058-8825-bc3f38f5210f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="27f21e744dd3fddc57345ffb4fd740de" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010092D0BEC079D6A24EA52990B6802652F9" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d524c98c6018639a2cf9265b59df29fb">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d3c0bec9-ac84-4257-9162-9ea5559110db" xmlns:ns3="57e54fb0-325f-4058-8825-bc3f38f5210f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fdef33c50015d2b9015ed62fb0b93f11" ns2:_="" ns3:_="">
     <xsd:import namespace="d3c0bec9-ac84-4257-9162-9ea5559110db"/>
     <xsd:import namespace="57e54fb0-325f-4058-8825-bc3f38f5210f"/>
     <xsd:element name="properties">
@@ -4558,6 +5409,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d3c0bec9-ac84-4257-9162-9ea5559110db">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="57e54fb0-325f-4058-8825-bc3f38f5210f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4568,11 +5430,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BCE969F-B16A-46A6-8A94-04ECF4103EFF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FDF08DF-9EDC-4386-BB8E-FEB8AEEDCD77}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B833A42E-865A-45D0-966F-990C1A59631E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BCE969F-B16A-46A6-8A94-04ECF4103EFF}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>